<commit_message>
full country and no country dataframes correct
</commit_message>
<xml_diff>
--- a/tests/data/some_country_data.xlsx
+++ b/tests/data/some_country_data.xlsx
@@ -7,9 +7,10 @@
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="energy_intensity_network" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="changes" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="metadata" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="time_B" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="power_B" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="changes" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="metadata" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -82,7 +83,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -90,6 +91,7 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -402,7 +404,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
@@ -507,7 +509,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>power_latop</t>
+          <t>power_A</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -564,7 +566,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>time_laptop</t>
+          <t>time_A</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -611,32 +613,54 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>energy_intensity_network</t>
+          <t>power_B</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>exp</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>20</v>
+          <t>interp</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>{"2020-01-01":10, "2031-06-01":9.5}</t>
+        </is>
       </c>
       <c r="F4" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1</v>
+        <v>4</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>42522</v>
+        <v>43617</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>kWh/GB</t>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="P4" s="3" t="inlineStr">
+        <is>
+          <t>what does it mean? How do collect this info?</t>
+        </is>
+      </c>
+      <c r="Q4" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="R4" s="3" t="inlineStr">
+        <is>
+          <t>power draw of laptop</t>
         </is>
       </c>
       <c r="S4" t="n">
@@ -646,22 +670,29 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>bitrate_laptop</t>
+          <t>time_B</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>exp</t>
-        </is>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>40000000</v>
+          <t>interp</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>{"2020-01-01":100, "2031-06-01":95}</t>
+        </is>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="H5" t="n">
         <v>0.05</v>
@@ -669,9 +700,14 @@
       <c r="I5" s="2" t="n">
         <v>43617</v>
       </c>
-      <c r="J5" s="3" t="inlineStr">
-        <is>
-          <t>bps</t>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>minute</t>
+        </is>
+      </c>
+      <c r="Q5" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
         </is>
       </c>
       <c r="S5" t="n">
@@ -679,39 +715,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>carbon_intensity</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>exp</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F6" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>43617</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>kg/kWh</t>
-        </is>
-      </c>
-      <c r="S6" t="n">
-        <v>5</v>
-      </c>
+      <c r="I6" s="2" t="n"/>
     </row>
     <row r="7">
       <c r="I7" s="2" t="n"/>
@@ -730,7 +734,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:G3"/>
+      <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -778,20 +782,22 @@
           <t>UK</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>20</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>{"2020-01-01":100, "2031-06-01":95}</t>
+        </is>
       </c>
       <c r="D2" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>6</v>
+        <v>0.05</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -800,20 +806,127 @@
           <t>DE</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>20</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>{"2020-01-01":100, "2031-06-01":95}</t>
+        </is>
       </c>
       <c r="D3" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G3" t="n">
-        <v>7</v>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>region</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>scenario</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ref value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>mean growth</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>initial_value_proportional_variation</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>variability growth</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>{"2020-01-01":10, "2031-06-01":9.5}</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>{"2020-01-01":10, "2031-06-01":9.5}</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="G3" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -821,7 +934,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -852,7 +965,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>